<commit_message>
:pencil: DE white belt training
</commit_message>
<xml_diff>
--- a/internalContent/DETraining/DXCUForms/Badge Creation Template 19-15-03.xlsx
+++ b/internalContent/DETraining/DXCUForms/Badge Creation Template 19-15-03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dxcportal-my.sharepoint.com/personal/rpetrova_dxc_com/Documents/P_Badges/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DXCWork\OneDrive - DXC Production\Projects\DXC\Digital Explorer\gitRepo\Digital-Explorer-Specs\internalContent\DETraining\DXCUForms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D799E038-BD9A-4EC7-A882-832EC05128CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{D799E038-BD9A-4EC7-A882-832EC05128CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3CB96998-9287-497D-B934-577C9D089323}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11535" windowHeight="5955" xr2:uid="{214306FA-6240-4162-BEEB-E71F35896C7E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{214306FA-6240-4162-BEEB-E71F35896C7E}"/>
   </bookViews>
   <sheets>
     <sheet name="START HERE Type and Image" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
   <si>
     <t>Go through the steps below to request your badge to appear on DXC University Saba</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Only Internal</t>
   </si>
   <si>
-    <t>Minor Competency Badge</t>
-  </si>
-  <si>
     <t>Sell</t>
   </si>
   <si>
@@ -233,45 +230,12 @@
     <t>Industry</t>
   </si>
   <si>
-    <t>The training you need to complete to get this badge will help you apply industry awareness to client solutions. It is appropriate for industry aligned solutioning professionals and individuals working in a client facing role.  Estimated time to earn the badge - 10 hours.</t>
-  </si>
-  <si>
-    <t>Industry Foundation Curriculum</t>
-  </si>
-  <si>
-    <t>10hrs</t>
-  </si>
-  <si>
-    <t>Complete the Industry Foundation Curriculum</t>
-  </si>
-  <si>
-    <t>Completion of the Industry Foundation Curriculum</t>
-  </si>
-  <si>
-    <t>Foundation</t>
-  </si>
-  <si>
-    <t>Yes, Industry Professional, Industry Master, Industry Grandmaster</t>
-  </si>
-  <si>
     <t>Attached</t>
   </si>
   <si>
-    <t>Apply Industry Awareness to client solutions</t>
-  </si>
-  <si>
-    <t>Badge attained by Industry aligned Solutioning Professionals</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>Industry Foundation</t>
-  </si>
-  <si>
-    <t>deborah-lynne.hallett@dxc.com; gancheva@dxc.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shows acquisition of a skill or knowledge at a basic level. Verified by in-built course knowledge checks, exams, practical assignments. </t>
   </si>
   <si>
@@ -341,9 +305,6 @@
     <t xml:space="preserve">Enter the number of the Courses/Curricula/Certifications in Saba to which the badge will be linked </t>
   </si>
   <si>
-    <t>000000000004325</t>
-  </si>
-  <si>
     <t>Describe the target group for your badge: eg. Client facing professionals, delivery lead, data engineers etc.</t>
   </si>
   <si>
@@ -357,6 +318,33 @@
   </si>
   <si>
     <t xml:space="preserve">2. DEVELOP &amp; SEND THE IMAGE TO DXC UNIVERSITY LEARNING OPERATIONS </t>
+  </si>
+  <si>
+    <t>DXC Digital Explorer White Belt</t>
+  </si>
+  <si>
+    <t>davidstevens@dxc.com</t>
+  </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>Complete the DXC Digital Explorer White Belt Curriculum</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Completion the DXC Digital Explorer White Belt Curriculum</t>
+  </si>
+  <si>
+    <t>Number of badges awarded</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>DXC Digital Explorer - White Belt</t>
   </si>
 </sst>
 </file>
@@ -560,7 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -571,9 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -600,19 +585,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -621,6 +599,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -955,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4D2947-CB9C-4DFB-BE9E-9D1D46D8977B}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
+      <c r="A2" s="20"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
     </row>
@@ -997,8 +981,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
-        <v>105</v>
+      <c r="B7" s="24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1020,17 +1004,17 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
-        <v>106</v>
+      <c r="B13" s="24" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>108</v>
+      <c r="A15" s="19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="1"/>
@@ -1056,7 +1040,7 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="1"/>
@@ -1070,10 +1054,10 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="1"/>
@@ -1086,7 +1070,7 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1138,7 +1122,7 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="1"/>
@@ -1152,11 +1136,11 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="29" t="s">
-        <v>85</v>
+      <c r="B25" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1168,11 +1152,11 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>86</v>
+      <c r="B26" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1196,8 +1180,8 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
-        <v>107</v>
+      <c r="A28" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1229,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACD82F0-6945-45EC-A9A6-2AEBC47363DD}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1250,52 +1234,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="23"/>
+      <c r="A1" s="21"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="25" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
     </row>
     <row r="7" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1308,30 +1292,30 @@
         <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>99</v>
+      <c r="H7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L7" s="5" t="s">
+      <c r="K7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="M7" s="3" t="s">
@@ -1349,341 +1333,320 @@
       <c r="Q7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S7" s="5" t="s">
+      <c r="S7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="7" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="G9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="S9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="S8" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
+      <c r="C19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1693,41 +1656,35 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="mailto:ldops@dxc.com?subject=Badge%20Creation%20Request" xr:uid="{6FFA2FFE-B954-446A-906F-2DD9FC5DEB8A}"/>
-    <hyperlink ref="B9" r:id="rId2" display="deborah-lynne.hallett@dxc.com" xr:uid="{E2165DC2-33B6-49A3-8150-7ADC1CA44814}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{6940FF84-948F-4C86-877F-451A468AC5C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C349191C-FD93-4885-AC65-DBBB3509104E}">
           <x14:formula1>
             <xm:f>'Lists DO NOT DELETE'!$A$3:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C20</xm:sqref>
+          <xm:sqref>C9:C19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA309C57-F756-447B-8DF7-3EC70CC31555}">
           <x14:formula1>
             <xm:f>'Lists DO NOT DELETE'!$D$3:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E9:E19</xm:sqref>
+          <xm:sqref>E9:E18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E7AD0A0-43F1-4444-B0A3-89567FBCDFC2}">
           <x14:formula1>
             <xm:f>'Lists DO NOT DELETE'!$E$3:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F9:F19</xm:sqref>
+          <xm:sqref>F9:F18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6280EECF-0F39-45C4-8923-10E492BA74E4}">
           <x14:formula1>
             <xm:f>'Lists DO NOT DELETE'!$B$3:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D9:D19</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED7688BF-2F8A-4B52-A9E3-2B79B68A4A79}">
-          <x14:formula1>
-            <xm:f>'C:\Users\rpetrova2\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\085BI3K6\[Copy of Badge Creation Template (003).xlsx]Lists DO NOT DELETE'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C9</xm:sqref>
+          <xm:sqref>D9:D18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1745,130 +1702,129 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="15" style="19" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="19" t="s">
+      <c r="F4" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="31" t="s">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="19" t="s">
+      <c r="F6" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="27"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1878,21 +1834,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010015D688BCB0AAEA49B5B2D36D061AC698" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a252bf2c5aae596da366669542fdf958">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="473b9712-6dda-4ded-8bae-2521c976cfd5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11187221a23b5c9f7dc2e83becce07a4" ns2:_="">
     <xsd:import namespace="473b9712-6dda-4ded-8bae-2521c976cfd5"/>
@@ -2030,31 +1971,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D46635-C466-4EF8-A72A-3C514419DFFA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="473b9712-6dda-4ded-8bae-2521c976cfd5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796B1906-50CB-4713-B028-81E906971A56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C16BB339-63D3-41E1-8E9D-348E478F9679}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2070,4 +2002,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796B1906-50CB-4713-B028-81E906971A56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D46635-C466-4EF8-A72A-3C514419DFFA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="473b9712-6dda-4ded-8bae-2521c976cfd5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>